<commit_message>
changed excel table and diagram
</commit_message>
<xml_diff>
--- a/Actividad3.2/Tabla_alfabeto_automata.xlsx
+++ b/Actividad3.2/Tabla_alfabeto_automata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\Trabajos\Semestre 4 carrera\Implementacion MC\Implementacion_MC\Actividad3.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7E7B40-17BE-4B65-AAD3-6800D810DEB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B5FD1D-52A8-4F42-A781-26AE29C8BA16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14790" yWindow="240" windowWidth="13065" windowHeight="15225" xr2:uid="{4F61ECC4-2625-4953-B8E7-8799D45FCCB2}"/>
   </bookViews>
@@ -1019,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{216CC5F7-277E-4096-9540-C8627F683D6F}">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,8 +1171,8 @@
       <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>1</v>
+      <c r="E4" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>20</v>
@@ -1258,8 +1258,8 @@
       <c r="E6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>3</v>
+      <c r="F6" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>20</v>
@@ -1303,8 +1303,8 @@
       <c r="F7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="11" t="s">
-        <v>4</v>
+      <c r="G7" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>20</v>

</xml_diff>